<commit_message>
Refactored precedence from case statement to key/value pair struct array. Renaming of variables
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -351,9 +351,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added signage. Test case 3+1*-3 fails. To solve in next commit
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="10365" windowHeight="5415"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -15,9 +15,30 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>(2+2)*(2*2)^2</t>
+  </si>
+  <si>
+    <t>1*(2*2)^2</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -26,12 +47,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -43,13 +70,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -349,26 +380,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
         <f>1+4*2-4^2+2^2^2*2+3-1</f>
         <v>27</v>
       </c>
-      <c r="E1">
-        <f>2*--++--++-+-27</f>
-        <v>54</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="B1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <f>((1+3-2/2)*(2^2^2)^2+1)*2^2-1</f>
         <v>3075</v>
+      </c>
+      <c r="B2">
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <f>3+(2+(3*2)*2+(2^2)--4)</f>
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <f>1*(2^2^2)^2+1</f>
+        <v>257</v>
+      </c>
+      <c r="B4">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <f>(1)*(2^2^2)^2+1</f>
+        <v>257</v>
+      </c>
+      <c r="B5">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <f>(1+1)*(2^2^2)^2+1</f>
+        <v>513</v>
+      </c>
+      <c r="B6">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <f>(1+1)*(3^3^2)^2+1</f>
+        <v>1062883</v>
+      </c>
+      <c r="B7">
+        <v>1062883</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3^2-4^2</f>
+        <v>185</v>
+      </c>
+      <c r="B8">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3</f>
+        <v>-63</v>
+      </c>
+      <c r="B9">
+        <v>-75</v>
+      </c>
+      <c r="L9">
+        <f>3*++--3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f>3+(1)*+-+----3</f>
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f>3+(1)*+-+--3</f>
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f>3+1*+-+--3</f>
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f>3+1*+--3</f>
+        <v>6</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f>3+1*-3</f>
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="23" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F23" t="s">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f>(2+2)*(2*2)^2</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="G24">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="26" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <f>1*(2*2)^2</f>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Complete signage functionality added. Parenthesis removed. Yet to test
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="10365" windowHeight="5415"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="10365" windowHeight="5415" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -382,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -556,12 +556,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>1-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>1+1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>1--1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f>1+-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f>1-1</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Complete parenthesis functionality with option to add +'s and -'s after opening bracket
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -58,8 +58,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="187" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -77,7 +78,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,6 +88,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -104,11 +111,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="187" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -414,109 +423,74 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="1">
+      <c r="A1" s="3">
         <f>1+4*2-4^2+2^2^2*2+3-1</f>
         <v>27</v>
       </c>
-      <c r="B1">
-        <v>27</v>
-      </c>
-      <c r="E1" s="1">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <f>((1+3-2/2)*(2^2^2)^2+1)*2^2-1</f>
+        <v>3075</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <f>1+4*2-4*2+2*2*2*2+3-1</f>
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <f>((1+3-2/2)*(2^2^2)^2+1)*2^2-1</f>
-        <v>3075</v>
-      </c>
-      <c r="B2">
-        <v>3075</v>
-      </c>
-      <c r="E2" s="1">
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <f>1+4*--2-4*+-+-2+2*--2*2*2+3-++-+--1</f>
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <f>((1+3-2/2)*(2^2^2)^2+1)*2^2-1</f>
-        <v>3075</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <f>3+(2+(3*2)*2+(2^2)--4)</f>
         <v>25</v>
       </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <f>1*(2^2^2)^2+1</f>
         <v>257</v>
       </c>
-      <c r="B5">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <f>(1)*(2^2^2)^2+1</f>
         <v>257</v>
       </c>
-      <c r="B6">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <f>((1+1)*(2^2^2)^2+(1--+((1+1)*4)))</f>
         <v>521</v>
       </c>
-      <c r="B7">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <f>(1+1)*(3^3^2)^2+1</f>
         <v>1062883</v>
       </c>
-      <c r="B8">
-        <v>1062883</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
         <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3^2-4^2</f>
         <v>185</v>
-      </c>
-      <c r="B9">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3</f>
-        <v>-63</v>
-      </c>
-      <c r="B10">
-        <v>-75</v>
       </c>
       <c r="L10">
         <f>3*++--3</f>
@@ -524,69 +498,55 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="3">
+        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3</f>
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <f>3+(1)*+-+----3</f>
         <v>0</v>
       </c>
-      <c r="B11">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f>3+(1)*+-+--3</f>
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>-12</v>
-      </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f>3+1*+-+--3</f>
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>-12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <f>3+1*+--3</f>
-        <v>6</v>
-      </c>
-      <c r="B14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A13" s="3">
         <f>3+1*-3</f>
         <v>0</v>
       </c>
-      <c r="B15">
-        <v>-12</v>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <f>+--+((1*+-7)^2)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <f>+--+((1*+-7)^---2)</f>
+        <v>2.0408163265306121E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <f>--(+-(1+3-2/2)*(2^2^2)^2+1)*2^2-1+(1*(1-3))</f>
+        <v>-3071</v>
       </c>
     </row>
     <row r="24" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>0</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="3">
         <f>(2+2)*(2*2)^2</f>
         <v>64</v>
-      </c>
-    </row>
-    <row r="25" spans="6:7" x14ac:dyDescent="0.25">
-      <c r="G25">
-        <v>256</v>
       </c>
     </row>
     <row r="27" spans="6:7" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>1</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="3">
         <f>1*(2*2)^2</f>
         <v>16</v>
       </c>
@@ -612,7 +572,7 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Regressed back to basic functionality except for multiple + and - before numbers
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="10365" windowHeight="5415"/>
+    <workbookView xWindow="240" yWindow="165" windowWidth="10365" windowHeight="5355" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>(2+2)*(2*2)^2</t>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t>1++++1</t>
+  </si>
+  <si>
+    <t>Arithmetic Precedence</t>
   </si>
 </sst>
 </file>
@@ -60,7 +64,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="187" formatCode="0.000000"/>
+    <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -111,13 +115,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="187" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -422,9 +432,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -533,7 +541,19 @@
         <v>-3071</v>
       </c>
     </row>
-    <row r="24" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <f>-(1+3-2/2)*(2^2^2)^2+1*2^2-1+(1*(1-3))</f>
+        <v>-767</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f>1+4+2-4+2+2^2^2-2+3-1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F24" t="s">
         <v>0</v>
       </c>
@@ -542,7 +562,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F27" t="s">
         <v>1</v>
       </c>
@@ -631,4 +651,192 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1">
+        <f>1+4*2-4^2+2^2^2*2+3-1</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="9">
+        <f>((1+3-2/2)*(2^(2^2+2))^2+1)*2^2-1</f>
+        <v>49155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <f>1+4*2-4*2+2*2*2*2+3-1</f>
+        <v>19</v>
+      </c>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B4" s="6">
+        <f>1+4*--2-4*+-+-2+2*--2*2*2+3-++-+--1</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <f>3+(2+(3*2)*2+(2^2)-4)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <f>1*(2^2^2)^2+1</f>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <f>(1)*(2^2^2)^2+1</f>
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <f>((1+1)*(2^2^2)^2+(1--+((1+1)*4)))</f>
+        <v>521</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="7">
+        <f>(1+1)*(3^3^2)^2+1</f>
+        <v>1062883</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="6">
+        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3^2-4^2</f>
+        <v>185</v>
+      </c>
+      <c r="M10">
+        <f>3*++--3</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3</f>
+        <v>-63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="6">
+        <f>3+(1)*+-+----3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="6">
+        <f>3+1*-3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="6">
+        <f>+--+((1*+-7)^2)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <f>+--+((1*+-7)^---2)</f>
+        <v>2.0408163265306121E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B16" s="6">
+        <f>--(+-(1+3-2/2)*(2^2^2)^2+1)*2^2-1+(1*(1-3))</f>
+        <v>-3071</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="6">
+        <f>-(1+3-2/2)*(2^2^2)^2+1*2^2-1+(1*(1-3))</f>
+        <v>-767</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="6">
+        <f>(1+3-2/2)*(2^2^2)^2+1*2^2-1</f>
+        <v>771</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <f>1+3-2/2*2^2^2^2+1*2^2-1</f>
+        <v>-249</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <f>(((-(1+1))*(2^2^2)^2+(-1-(-(1+1)*4))-1*2^3)+5)</f>
+        <v>-508</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Multiple signage except for * or / followed by +'s and -'s
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>(2+2)*(2*2)^2</t>
   </si>
@@ -55,7 +55,22 @@
     <t>1++++1</t>
   </si>
   <si>
-    <t>Arithmetic Precedence</t>
+    <t>All Operator Precedence</t>
+  </si>
+  <si>
+    <t>With opening signs in beginning and parenthesis</t>
+  </si>
+  <si>
+    <t>With brackets</t>
+  </si>
+  <si>
+    <t>With double Brackets opening and close</t>
+  </si>
+  <si>
+    <t>Multiple signage</t>
+  </si>
+  <si>
+    <t>Multiple signage following sign</t>
   </si>
 </sst>
 </file>
@@ -655,15 +670,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
@@ -672,134 +687,93 @@
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="9">
         <f>1+4*2-4^2+2^2^2*2+3-1</f>
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
       <c r="B2" s="9">
+        <f>(1+3-2/2*(2^2^2+2)^2+1)*2^2-1</f>
+        <v>-1277</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="9">
         <f>((1+3-2/2)*(2^(2^2+2))^2+1)*2^2-1</f>
         <v>49155</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="1">
-        <f>1+4*2-4*2+2*2*2*2+3-1</f>
-        <v>19</v>
-      </c>
-      <c r="F3" s="6"/>
-    </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="6">
-        <f>1+4*--2-4*+-+-2+2*--2*2*2+3-++-+--1</f>
-        <v>21</v>
-      </c>
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="9">
+        <f>-(-(1+3-2/2)*(2^(2^2+2))^2+1)*2^2-1</f>
+        <v>49147</v>
+      </c>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="1">
-        <f>3+(2+(3*2)*2+(2^2)-4)</f>
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="9">
+        <f>+--+(+-+((-+-(1+-1))*(2^2^2)^2+(-1-(-(-+-1+1)*4))-1*2^3)+5)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="1">
-        <f>1*(2^2^2)^2+1</f>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="1">
-        <f>(1)*(2^2^2)^2+1</f>
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="1">
-        <f>((1+1)*(2^2^2)^2+(1--+((1+1)*4)))</f>
-        <v>521</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
-        <f>(1+1)*(3^3^2)^2+1</f>
-        <v>1062883</v>
+      <c r="B6" s="9">
+        <f>+--+(+-+((-+-(1+-1))*(2^2^2)^2*-(-1-(-(-+-1+1)*4))-1*2^-3)+5)</f>
+        <v>5.125</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3^2-4^2</f>
-        <v>185</v>
-      </c>
-      <c r="M10">
+      <c r="B10" s="7"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="6"/>
+      <c r="M11">
         <f>3*++--3</f>
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <f>3+(2+(3*2)*2+(2^2)--4)*+-+----3</f>
-        <v>-63</v>
-      </c>
-    </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <f>3+(1)*+-+----3</f>
-        <v>0</v>
-      </c>
+      <c r="B12" s="6"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <f>3+1*-3</f>
-        <v>0</v>
-      </c>
+      <c r="B13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
-        <f>+--+((1*+-7)^2)</f>
-        <v>49</v>
-      </c>
+      <c r="B14" s="6"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B15" s="8">
-        <f>+--+((1*+-7)^---2)</f>
-        <v>2.0408163265306121E-2</v>
-      </c>
+      <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="6">
-        <f>--(+-(1+3-2/2)*(2^2^2)^2+1)*2^2-1+(1*(1-3))</f>
-        <v>-3071</v>
-      </c>
+      <c r="B16" s="8"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="6">
-        <f>-(1+3-2/2)*(2^2^2)^2+1*2^2-1+(1*(1-3))</f>
-        <v>-767</v>
-      </c>
+      <c r="B17" s="6"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="6">
-        <f>(1+3-2/2)*(2^2^2)^2+1*2^2-1</f>
-        <v>771</v>
-      </c>
+      <c r="B18" s="6"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="6">
-        <f>1+3-2/2*2^2^2^2+1*2^2-1</f>
-        <v>-249</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="1">
-        <f>(((-(1+1))*(2^2^2)^2+(-1-(-(1+1)*4))-1*2^3)+5)</f>
-        <v>-508</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
+      <c r="B19" s="6"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="G24" s="6"/>
@@ -836,6 +810,11 @@
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
     </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
End of retrying refactoring branch
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -130,7 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -138,7 +138,6 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -673,7 +672,7 @@
   <dimension ref="A1:M31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +686,7 @@
       <c r="A1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="8">
         <f>1+4*2-4^2+2^2^2*2+3-1</f>
         <v>27</v>
       </c>
@@ -696,7 +695,7 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="8">
         <f>(1+3-2/2*(2^2^2+2)^2+1)*2^2-1</f>
         <v>-1277</v>
       </c>
@@ -705,7 +704,7 @@
       <c r="A3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <f>((1+3-2/2)*(2^(2^2+2))^2+1)*2^2-1</f>
         <v>49155</v>
       </c>
@@ -714,7 +713,7 @@
       <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <f>-(-(1+3-2/2)*(2^(2^2+2))^2+1)*2^2-1</f>
         <v>49147</v>
       </c>
@@ -724,22 +723,25 @@
       <c r="A5" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="9">
-        <f>+--+(+-+((-+-(1+-1))*(2^2^2)^2+(-1-(-(-+-1+1)*4))-1*2^3)+5)</f>
-        <v>6</v>
+      <c r="B5" s="8">
+        <f>+--+(+-+((-+-(1+--1))*(2^2^2)^2+(-1-(-(-+-1+-1)*4))-1*2^3)+--5)</f>
+        <v>-498</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <f>+--+(+-+((-+-(1+-1))*(2^2^2)^2*-(-1-(-(-+-1+1)*4))-1*2^-3)+5)</f>
         <v>5.125</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="7"/>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f>(-1-(-(-+-1+1)*4))-1*2^-3</f>
+        <v>6.875</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="6"/>
@@ -749,7 +751,13 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
+      <c r="B12">
+        <f>1*2^-3</f>
+        <v>0.125</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="6"/>
@@ -761,7 +769,7 @@
       <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="8"/>
+      <c r="B16" s="7"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="6"/>

</xml_diff>